<commit_message>
More refrigerant ph diagrams added
</commit_message>
<xml_diff>
--- a/Inputs/Boundary_Conditions/Boundary_Conditions.xlsx
+++ b/Inputs/Boundary_Conditions/Boundary_Conditions.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Abhay\Automotive Thermal management\Python\VapourCompression\Inputs\Boundary_Conditions\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Abhay\Automotive Thermal management\Python\VapourCompressionPython\Inputs\Boundary_Conditions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5C477B7-AB65-44CD-ADC3-42DC192488C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5AE7CD4-45D9-44D8-ABC0-01930DFB940C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{33975EF2-86F2-48AE-AD69-7F1DACC0CD12}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
   <si>
     <t>Parameter</t>
   </si>
@@ -83,13 +83,34 @@
   </si>
   <si>
     <t>R12</t>
+  </si>
+  <si>
+    <t>R1233zd</t>
+  </si>
+  <si>
+    <t>R152A</t>
+  </si>
+  <si>
+    <t>R410A</t>
+  </si>
+  <si>
+    <t>R717</t>
+  </si>
+  <si>
+    <t>R718</t>
+  </si>
+  <si>
+    <t>R32</t>
+  </si>
+  <si>
+    <t>R744</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -101,6 +122,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1" tint="0.499984740745262"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -147,7 +175,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -160,6 +188,7 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -477,7 +506,7 @@
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -499,7 +528,7 @@
         <v>13</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -513,7 +542,7 @@
         <v>9</v>
       </c>
       <c r="B4" s="2">
-        <v>30</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -551,7 +580,7 @@
         <v>9</v>
       </c>
       <c r="B9" s="2">
-        <v>30</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -621,7 +650,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{6F880EB5-D9AC-4F2D-A4BB-DB6521DF48E3}">
           <x14:formula1>
-            <xm:f>Lists!$B$11:$B$17</xm:f>
+            <xm:f>Lists!$B$11:$B$13</xm:f>
           </x14:formula1>
           <xm:sqref>B2</xm:sqref>
         </x14:dataValidation>
@@ -633,10 +662,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{627C4366-1659-4C00-A264-BB5D9C9E9195}">
-  <dimension ref="B10:B14"/>
+  <dimension ref="B10:B21"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -661,12 +690,47 @@
     </row>
     <row r="13" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B14" s="8" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
+    <row r="15" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B15" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B16" s="8" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B21" s="8" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>